<commit_message>
Finished func load_balance_quarterly v2
</commit_message>
<xml_diff>
--- a/output.xlsx
+++ b/output.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\SeboB\Desktop\Data Science\Code\FullStackTradingApp\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{99B7B0EA-48BD-4D0A-9A96-E48FAB7CE519}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{19298909-86C1-42B0-9FE7-D583DFF3E0ED}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15840" activeTab="1" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -9169,8 +9169,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0100-000000000000}">
   <dimension ref="A1:AO122"/>
   <sheetViews>
-    <sheetView tabSelected="1" zoomScaleNormal="100" workbookViewId="0">
-      <selection sqref="A1:XFD1048576"/>
+    <sheetView tabSelected="1" topLeftCell="A100" zoomScaleNormal="100" workbookViewId="0">
+      <selection activeCell="G20" sqref="G20"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="9.140625" defaultRowHeight="15" x14ac:dyDescent="0.25"/>

</xml_diff>